<commit_message>
v0.38.18 	! Several tests added in the background (Not part of the package yet) to ensure a safer release 		The (future) goal is to create tests small enough to fit with the package for the same failure modes 	! Fixes #82 in github as well as removing the fail for negative decimal rounding numbers inferred from scientific notiation 	! Addresses #81 in github with safer string searching 	! Addresses #80 in github by Manually building this package on my system and then running the Spreadsheet::Read (master) 		tests after.  Long term I would like to import more of that testing to this package. 	! Addresses #79 in github with by allowing for EOF flags to add this and only use the value where available 		Still needs a test added to the test suit 	! Addresses #78 in github with by substituting the values from the sheet where no row span is provided 		Still needs a test added to the test suit
</commit_message>
<xml_diff>
--- a/t/test_files/hidden_format_test.xlsx
+++ b/t/test_files/hidden_format_test.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>E421745</t>
+  </si>
+  <si>
+    <t>121E22671</t>
   </si>
 </sst>
 </file>
@@ -59,10 +62,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -443,6 +447,16 @@
         <v>5.0000000000000004E-19</v>
       </c>
     </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>